<commit_message>
output folder and limited tc functionality added
</commit_message>
<xml_diff>
--- a/notebooks/SampleTestData1.xlsx
+++ b/notebooks/SampleTestData1.xlsx
@@ -784,13 +784,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -837,7 +837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>654</v>
       </c>
@@ -869,7 +869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>53</v>
       </c>
@@ -901,7 +901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>903</v>
       </c>
@@ -997,7 +997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>900</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>555</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>637</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>669</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>281</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>819</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>579</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>141</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>349</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>403</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>846</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>612</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>171</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>794</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>698</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>57</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>219</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>139</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>67</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>118</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>173</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>91</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
         <v>675</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>584</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>596</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>847</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>942</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
         <v>189</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
         <v>406</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
         <v>309</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
         <v>963</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
         <v>252</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
         <v>38</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
         <v>743</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
         <v>199</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
         <v>878</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
         <v>353</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
         <v>487</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
         <v>640</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
         <v>992</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
         <v>448</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
         <v>226</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
         <v>973</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
         <v>264</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
         <v>949</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
         <v>12</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="67" s="3" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
         <v>654</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
         <v>903</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" s="3" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
         <v>654</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
         <v>903</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
         <v>654</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
         <v>903</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
         <v>38</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
         <v>67</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
         <v>654</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
         <v>579</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
         <v>846</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
         <v>67</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
         <v>654</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
         <v>579</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
         <v>846</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="n">
         <v>67</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="n">
         <v>654</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
         <v>900</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="n">
         <v>900</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="n">
         <v>900</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="n">
         <v>637</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="n">
         <v>669</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="n">
         <v>171</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="n">
         <v>794</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="n">
         <v>698</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="n">
         <v>57</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="n">
         <v>900</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="n">
         <v>637</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="n">
         <v>669</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="n">
         <v>171</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="n">
         <v>794</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="n">
         <v>698</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="n">
         <v>57</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="n">
         <v>819</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="n">
         <v>141</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="n">
         <v>819</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="n">
         <v>141</v>
       </c>
@@ -4454,13 +4454,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H114">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="No"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H114"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>